<commit_message>
added transactions and draft
</commit_message>
<xml_diff>
--- a/WeeklyPlayerScores.xlsx
+++ b/WeeklyPlayerScores.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwest\code\mfl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B344B16C-CCCE-42CC-B75E-791FE470D6BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384E11B-20B4-482F-A911-E8C90F536DD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="456" yWindow="456" windowWidth="19332" windowHeight="11388" xr2:uid="{18C86054-C21F-4DD2-8BED-143C0A08A3C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WeeklyPlayerScores" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>